<commit_message>
Framework Code Refractor Inprogress
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumPageObjectModelFrameworkExtended\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E795C7F-300B-4754-BE84-F301F20D33B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE1AE23-AA01-4261-B09B-81310C4E083C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>RunMode</t>
   </si>
@@ -448,7 +448,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,37 +486,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C39480-F02B-40BC-AAFB-DAA923AC03BA}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Refactor - Dry Run Login Test, Issue Fixed. Dry Run Passed.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumPageObjectModelFrameworkExtended\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Intellij_Env\SeleniumTestFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE1AE23-AA01-4261-B09B-81310C4E083C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE15601-C4AD-4678-8E5C-19E33F176CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C39480-F02B-40BC-AAFB-DAA923AC03BA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code Refactor - Test Execution RunMode Updated.TestListener code updated. TimeSheet Functionality automation InProgress.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Intellij_Env\SeleniumTestFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE15601-C4AD-4678-8E5C-19E33F176CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4373DE30-3D9F-41A2-B347-1CB936517AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>RunMode</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>admin12</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -406,7 +412,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +441,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,6 +485,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -489,7 +506,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code Refactor - TimeSheet Functionality automation InProgress.Fixed the Sync up issue. Code Updated InProgress.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Intellij_Env\SeleniumTestFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4373DE30-3D9F-41A2-B347-1CB936517AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8730C1CD-3998-4E12-8B08-858B880EBCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
     <sheet name="LoginPageTest" sheetId="1" r:id="rId2"/>
     <sheet name="AdminPageTest" sheetId="5" r:id="rId3"/>
+    <sheet name="TimePageTest" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>RunMode</t>
   </si>
@@ -69,6 +70,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>TimePageTest</t>
   </si>
 </sst>
 </file>
@@ -409,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441ED292-DA54-48C6-B808-307C6EE8D48C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +437,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -442,6 +446,14 @@
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -453,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,4 +567,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3977DC-0C87-46C4-8425-FF285ED595B4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code Refactor - WaitHandler Code Update InProgress. General Code Restructure also InProgress.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Intellij_Env\SeleniumTestFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8730C1CD-3998-4E12-8B08-858B880EBCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F005CAD-02AB-49E7-B659-8C9532E64307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +437,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -445,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -466,7 +466,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code Refactor - WaitHandler Code Update Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Intellij_Env\SeleniumTestFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9149BE-CF8B-41CA-894B-513105240FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416A5554-8EAF-4DBF-A361-F8401FE04B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
     <sheet name="LoginPageTest" sheetId="1" r:id="rId2"/>
     <sheet name="AdminPageTest" sheetId="5" r:id="rId3"/>
-    <sheet name="TimePageTest" sheetId="6" r:id="rId4"/>
+    <sheet name="TimesheetPageTest" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>RunMode</t>
   </si>
@@ -72,7 +72,13 @@
     <t>N</t>
   </si>
   <si>
-    <t>TimePageTest</t>
+    <t>TimesheetPageTest</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Attendance</t>
   </si>
 </sst>
 </file>
@@ -416,7 +422,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +524,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,20 +577,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3977DC-0C87-46C4-8425-FF285ED595B4}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -592,10 +600,13 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -603,6 +614,9 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Refactor - EncryptionManager utility added to handle the password. Updated the Test scripts.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Intellij_Env\SeleniumTestFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416A5554-8EAF-4DBF-A361-F8401FE04B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C045BDB-8DE4-472A-898A-23C5B87BF891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>TestCaseName</t>
   </si>
   <si>
-    <t>admin12</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -79,6 +73,12 @@
   </si>
   <si>
     <t>Attendance</t>
+  </si>
+  <si>
+    <t>gG+7Twxtcof2boCuiDPlzA==</t>
+  </si>
+  <si>
+    <t>/bbmmvb4w8JDpN0RgERT3w==</t>
   </si>
 </sst>
 </file>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441ED292-DA54-48C6-B808-307C6EE8D48C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +432,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -443,7 +443,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -451,15 +451,15 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -472,13 +472,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -494,10 +494,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -505,10 +505,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -524,13 +524,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -543,10 +543,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
@@ -554,16 +554,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -579,14 +579,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3977DC-0C87-46C4-8425-FF285ED595B4}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -600,7 +600,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -608,13 +608,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Code Refactor - Test Scripts, Page Classes code refactored for more readability.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Intellij_Env\SeleniumTestFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C045BDB-8DE4-472A-898A-23C5B87BF891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C558409B-D403-42CE-B2EB-647F2FA36284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +451,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -472,7 +472,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code Refactor - Browser Private Mode Launch Option Added.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Intellij_Env\SeleniumTestFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C558409B-D403-42CE-B2EB-647F2FA36284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44660CEB-F94F-4E8C-9CEE-F8484129A586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441ED292-DA54-48C6-B808-307C6EE8D48C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +451,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +511,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>